<commit_message>
fix: Remove experimental code
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="32720" windowHeight="14720"/>
+    <workbookView windowWidth="26380" windowHeight="14720"/>
   </bookViews>
   <sheets>
     <sheet name="access" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
   <si>
     <t>L1</t>
   </si>
@@ -34,6 +34,9 @@
     <t>GD_D93</t>
   </si>
   <si>
+    <t>JS_D93</t>
+  </si>
+  <si>
     <t>GD_CASA_01</t>
   </si>
   <si>
@@ -77,6 +80,21 @@
   </si>
   <si>
     <t>DX_IPQAM_03</t>
+  </si>
+  <si>
+    <t>JS_CASA_01</t>
+  </si>
+  <si>
+    <t>JS_CASA_02</t>
+  </si>
+  <si>
+    <t>JS_IPQAM_01</t>
+  </si>
+  <si>
+    <t>JS_IPQAM_02</t>
+  </si>
+  <si>
+    <t>JS_IPQAM_03</t>
   </si>
 </sst>
 </file>
@@ -1021,10 +1039,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33333333333333" defaultRowHeight="19" outlineLevelCol="1"/>
@@ -1061,7 +1079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" s="1" customFormat="1" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1089,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1111,7 +1129,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
@@ -1151,7 +1169,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1187,6 +1205,54 @@
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>